<commit_message>
Changing the distributions table
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
-  <si>
-    <t xml:space="preserve">title</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
+  <si>
+    <t xml:space="preserve">distr_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">param_title</t>
   </si>
   <si>
     <t xml:space="preserve">distr</t>
@@ -43,7 +46,10 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">Exponential Distribution / Rate Parametrization</t>
+    <t xml:space="preserve">Exponential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate</t>
   </si>
   <si>
     <t xml:space="preserve">exp</t>
@@ -64,31 +70,28 @@
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
-    <t xml:space="preserve">Exponential Distribution / Scale Parametrization</t>
+    <t xml:space="preserve">Scale</t>
   </si>
   <si>
     <t xml:space="preserve">scale</t>
   </si>
   <si>
-    <t xml:space="preserve">Gamma Distribution / Rate Parametrization</t>
+    <t xml:space="preserve">Gamma</t>
   </si>
   <si>
     <t xml:space="preserve">gamma</t>
   </si>
   <si>
-    <t xml:space="preserve">Gamma Distribution / Scale Parametrization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generalized Gamma Distribution / Rate Parametrization</t>
+    <t xml:space="preserve">Generalized Gamma</t>
   </si>
   <si>
     <t xml:space="preserve">gengamma</t>
   </si>
   <si>
-    <t xml:space="preserve">Generalized Gamma Distribution / Scale Parametrization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geometric Distribution / Mean Parametrization</t>
+    <t xml:space="preserve">Geometric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean</t>
   </si>
   <si>
     <t xml:space="preserve">geom</t>
@@ -100,13 +103,16 @@
     <t xml:space="preserve">count</t>
   </si>
   <si>
-    <t xml:space="preserve">Geometric Distribution / Probabilistic Parametrization</t>
+    <t xml:space="preserve">Probabilistic</t>
   </si>
   <si>
     <t xml:space="preserve">prob</t>
   </si>
   <si>
-    <t xml:space="preserve">Multivariate Normal Distribution / Standard Parametrization</t>
+    <t xml:space="preserve">Multivariate Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard</t>
   </si>
   <si>
     <t xml:space="preserve">mnorm</t>
@@ -121,7 +127,10 @@
     <t xml:space="preserve">multi</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative Binomial Distribution / NB2 Parametrization</t>
+    <t xml:space="preserve">Negative Binomial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB2</t>
   </si>
   <si>
     <t xml:space="preserve">negbin</t>
@@ -130,16 +139,13 @@
     <t xml:space="preserve">nb2</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative Binomial Distribution / Probabilistic Parametrization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal Distribution / Standard Parametrization</t>
+    <t xml:space="preserve">Normal</t>
   </si>
   <si>
     <t xml:space="preserve">norm</t>
   </si>
   <si>
-    <t xml:space="preserve">Plackett-Luce Distribution / Standard Parametrization</t>
+    <t xml:space="preserve">Plackett-Luce</t>
   </si>
   <si>
     <t xml:space="preserve">pluce</t>
@@ -148,34 +154,31 @@
     <t xml:space="preserve">ranking</t>
   </si>
   <si>
-    <t xml:space="preserve">Poisson Distribution / Standard Parametrization</t>
+    <t xml:space="preserve">Poisson</t>
   </si>
   <si>
     <t xml:space="preserve">pois</t>
   </si>
   <si>
-    <t xml:space="preserve">Weibull Distribution / Rate Parametrization</t>
+    <t xml:space="preserve">Weibull</t>
   </si>
   <si>
     <t xml:space="preserve">weibull</t>
   </si>
   <si>
-    <t xml:space="preserve">Weibull Distribution / Scale Parametrization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zero-Inflated Geometric Distribution / Mean Parametrization</t>
+    <t xml:space="preserve">Zero-Inflated Geometric</t>
   </si>
   <si>
     <t xml:space="preserve">zigeom</t>
   </si>
   <si>
-    <t xml:space="preserve">Zero-Inflated Negative Binomial Distribution / NB2 Parametrization</t>
+    <t xml:space="preserve">Zero-Inflated Negative Binomial</t>
   </si>
   <si>
     <t xml:space="preserve">zinegbin</t>
   </si>
   <si>
-    <t xml:space="preserve">Zero-Inflated Poisson Distribution / Standard Parametrization</t>
+    <t xml:space="preserve">Zero-Inflated Poisson</t>
   </si>
   <si>
     <t xml:space="preserve">zipois</t>
@@ -291,15 +294,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,74 +327,86 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>13</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,68 +414,77 @@
         <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,197 +501,224 @@
         <v>25</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>12</v>
+      <c r="F9" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,91 +726,103 @@
         <v>46</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>25</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the Bernoulli distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="57">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -46,6 +49,27 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
+    <t xml:space="preserve">Bernoulli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bernoulli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exponential</t>
   </si>
   <si>
@@ -61,12 +85,6 @@
     <t xml:space="preserve">duration</t>
   </si>
   <si>
-    <t xml:space="preserve">uni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
@@ -112,13 +130,7 @@
     <t xml:space="preserve">Multivariate Normal</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
     <t xml:space="preserve">mnorm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">std</t>
   </si>
   <si>
     <t xml:space="preserve">real</t>
@@ -289,18 +301,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -354,24 +370,24 @@
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>13</v>
@@ -380,134 +396,134 @@
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>14</v>
@@ -515,19 +531,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
@@ -536,56 +552,56 @@
         <v>14</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="F10" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="D11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>14</v>
@@ -593,77 +609,77 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>14</v>
@@ -674,22 +690,22 @@
         <v>44</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>45</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>14</v>
@@ -697,77 +713,77 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>14</v>
@@ -775,25 +791,25 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>14</v>
@@ -801,31 +817,58 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H21"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -833,5 +876,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the categorical distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,7 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="62">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -70,6 +71,27 @@
     <t xml:space="preserve">TRUE</t>
   </si>
   <si>
+    <t xml:space="preserve">Categorical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categorical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exponential</t>
   </si>
   <si>
@@ -85,9 +107,6 @@
     <t xml:space="preserve">duration</t>
   </si>
   <si>
-    <t xml:space="preserve">FALSE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scale</t>
   </si>
   <si>
@@ -134,9 +153,6 @@
   </si>
   <si>
     <t xml:space="preserve">real</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multi</t>
   </si>
   <si>
     <t xml:space="preserve">Negative Binomial</t>
@@ -310,13 +326,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -390,30 +406,30 @@
         <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
@@ -422,134 +438,134 @@
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="E9" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>14</v>
@@ -557,19 +573,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>13</v>
@@ -578,56 +594,56 @@
         <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>14</v>
@@ -635,77 +651,77 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>14</v>
@@ -713,25 +729,25 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>14</v>
@@ -739,77 +755,77 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="E19" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>14</v>
@@ -817,25 +833,25 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>14</v>
@@ -843,32 +859,58 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="C22" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="2" t="s">
+      <c r="E22" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H21"/>
+  <autoFilter ref="A1:H22"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding vector representation of categorical data
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,9 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="64">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -92,6 +93,15 @@
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
+    <t xml:space="preserve">Double Poisson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exponential</t>
   </si>
   <si>
@@ -135,9 +145,6 @@
   </si>
   <si>
     <t xml:space="preserve">mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">count</t>
   </si>
   <si>
     <t xml:space="preserve">Probabilistic</t>
@@ -326,13 +333,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -420,17 +427,17 @@
         <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
@@ -438,24 +445,24 @@
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
@@ -464,50 +471,50 @@
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>13</v>
@@ -516,24 +523,24 @@
         <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
@@ -542,24 +549,24 @@
         <v>21</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
@@ -568,30 +575,30 @@
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>14</v>
@@ -599,19 +606,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
@@ -620,56 +627,56 @@
         <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>14</v>
@@ -677,54 +684,54 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="D15" s="0" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -741,13 +748,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>14</v>
@@ -755,25 +762,25 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>14</v>
@@ -784,42 +791,42 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
@@ -828,7 +835,7 @@
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,16 +843,16 @@
         <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
@@ -862,16 +869,16 @@
         <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
@@ -888,29 +895,55 @@
         <v>60</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="2" t="s">
+      <c r="E23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H22"/>
+  <autoFilter ref="A1:H23"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding double Poisson distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,9 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$23</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="64">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -92,6 +93,15 @@
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
+    <t xml:space="preserve">Double Poisson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dpois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exponential</t>
   </si>
   <si>
@@ -135,9 +145,6 @@
   </si>
   <si>
     <t xml:space="preserve">mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">count</t>
   </si>
   <si>
     <t xml:space="preserve">Probabilistic</t>
@@ -326,13 +333,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -420,17 +427,17 @@
         <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
@@ -438,24 +445,24 @@
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
@@ -464,50 +471,50 @@
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>13</v>
@@ -516,24 +523,24 @@
         <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
@@ -542,24 +549,24 @@
         <v>21</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
@@ -568,30 +575,30 @@
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>14</v>
@@ -599,19 +606,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
@@ -620,56 +627,56 @@
         <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="C12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>14</v>
@@ -677,54 +684,54 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="D15" s="0" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -741,13 +748,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>14</v>
@@ -755,25 +762,25 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>14</v>
@@ -784,42 +791,42 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>28</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
@@ -828,7 +835,7 @@
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,16 +843,16 @@
         <v>56</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
@@ -862,16 +869,16 @@
         <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
@@ -888,29 +895,55 @@
         <v>60</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="2" t="s">
+      <c r="E23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H22"/>
+  <autoFilter ref="A1:H23"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the Student's t distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -12,8 +12,8 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$23</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">dist_table!$A$1:$H$21</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="66">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t xml:space="preserve">pois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student‘s t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
   </si>
   <si>
     <t xml:space="preserve">Weibull</t>
@@ -333,13 +339,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -817,16 +823,16 @@
         <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
@@ -835,21 +841,21 @@
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>29</v>
@@ -861,7 +867,7 @@
         <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,16 +875,16 @@
         <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
@@ -895,13 +901,13 @@
         <v>60</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>24</v>
@@ -921,13 +927,13 @@
         <v>62</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>24</v>
@@ -939,6 +945,32 @@
         <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding the Skellam distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,9 +11,9 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$23</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$24</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$22</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$26</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="71">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -54,13 +54,13 @@
     <t xml:space="preserve">Bernoulli</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard</t>
+    <t xml:space="preserve">Probabilistic</t>
   </si>
   <si>
     <t xml:space="preserve">bernoulli</t>
   </si>
   <si>
-    <t xml:space="preserve">std</t>
+    <t xml:space="preserve">prob</t>
   </si>
   <si>
     <t xml:space="preserve">binary</t>
@@ -96,9 +96,15 @@
     <t xml:space="preserve">Double Poisson</t>
   </si>
   <si>
+    <t xml:space="preserve">Mean</t>
+  </si>
+  <si>
     <t xml:space="preserve">dpois</t>
   </si>
   <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
     <t xml:space="preserve">count</t>
   </si>
   <si>
@@ -138,27 +144,21 @@
     <t xml:space="preserve">Geometric</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean</t>
-  </si>
-  <si>
     <t xml:space="preserve">geom</t>
   </si>
   <si>
-    <t xml:space="preserve">mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Probabilistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prob</t>
-  </si>
-  <si>
     <t xml:space="preserve">Multivariate Normal</t>
   </si>
   <si>
+    <t xml:space="preserve">Location-Sq-Scale</t>
+  </si>
+  <si>
     <t xml:space="preserve">mnorm</t>
   </si>
   <si>
+    <t xml:space="preserve">lss</t>
+  </si>
+  <si>
     <t xml:space="preserve">real</t>
   </si>
   <si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t xml:space="preserve">pois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skellam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skellam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
   </si>
   <si>
     <t xml:space="preserve">Student‘s t</t>
@@ -339,13 +354,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -433,16 +448,16 @@
         <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
@@ -456,19 +471,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
@@ -482,19 +497,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
@@ -508,19 +523,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>13</v>
@@ -534,19 +549,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="C8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
@@ -560,19 +575,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
@@ -586,19 +601,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>13</v>
@@ -612,19 +627,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
@@ -638,19 +653,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
@@ -664,16 +679,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>11</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>44</v>
@@ -702,7 +717,7 @@
         <v>48</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>13</v>
@@ -719,16 +734,16 @@
         <v>45</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>13</v>
@@ -745,13 +760,13 @@
         <v>49</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>44</v>
@@ -771,13 +786,13 @@
         <v>51</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>53</v>
@@ -797,16 +812,16 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
@@ -823,16 +838,16 @@
         <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
@@ -841,24 +856,24 @@
         <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="D20" s="0" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
@@ -867,24 +882,24 @@
         <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
@@ -898,19 +913,19 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
@@ -919,24 +934,24 @@
         <v>21</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
@@ -950,19 +965,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>13</v>
@@ -974,8 +989,60 @@
         <v>14</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H23"/>
+  <autoFilter ref="A1:H26"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Changing names of some distributions and parametrizations
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,9 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$26</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$24</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="73">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -153,13 +152,35 @@
     <t xml:space="preserve">Mean-Variance</t>
   </si>
   <si>
-    <t xml:space="preserve">mnorm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean_var</t>
+    <t xml:space="preserve">mvnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meanvar</t>
   </si>
   <si>
     <t xml:space="preserve">real</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Multivariate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Student‘s t</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">mvt</t>
   </si>
   <si>
     <t xml:space="preserve">Negative Binomial</t>
@@ -248,7 +269,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -276,6 +297,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -320,7 +346,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,6 +359,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,6 +372,15 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -354,13 +393,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -704,26 +743,26 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="D14" s="0" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>14</v>
@@ -731,16 +770,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>26</v>
@@ -749,36 +788,36 @@
         <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="D16" s="0" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,22 +825,22 @@
         <v>51</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>14</v>
@@ -809,25 +848,25 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="D18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F18" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>14</v>
@@ -838,42 +877,42 @@
         <v>56</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="D19" s="0" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
@@ -882,24 +921,24 @@
         <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>43</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
@@ -916,16 +955,16 @@
         <v>63</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>64</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
@@ -934,21 +973,21 @@
         <v>21</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>31</v>
@@ -960,7 +999,7 @@
         <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,16 +1007,16 @@
         <v>65</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>13</v>
@@ -994,13 +1033,13 @@
         <v>67</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>26</v>
@@ -1020,13 +1059,13 @@
         <v>69</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>70</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>26</v>
@@ -1041,14 +1080,40 @@
         <v>14</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H25"/>
+  <autoFilter ref="A1:H27"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding the mean-dispersion parametrization to the Skellam distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$25</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$28</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$26</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="75">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -161,23 +161,7 @@
     <t xml:space="preserve">real</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Multivariate </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Student‘s t</t>
-    </r>
+    <t xml:space="preserve">Multivariate Student‘s t</t>
   </si>
   <si>
     <t xml:space="preserve">mvt</t>
@@ -229,6 +213,12 @@
   </si>
   <si>
     <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean-Dispersion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meandisp</t>
   </si>
   <si>
     <t xml:space="preserve">Student‘s t</t>
@@ -269,7 +259,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -297,11 +287,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -359,7 +344,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -393,13 +378,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -929,13 +914,13 @@
         <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>62</v>
@@ -947,24 +932,24 @@
         <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
@@ -981,16 +966,16 @@
         <v>65</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>66</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
@@ -999,21 +984,21 @@
         <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>31</v>
@@ -1025,7 +1010,7 @@
         <v>21</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,16 +1018,16 @@
         <v>67</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>13</v>
@@ -1059,13 +1044,13 @@
         <v>69</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>70</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>26</v>
@@ -1085,13 +1070,13 @@
         <v>71</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>26</v>
@@ -1106,8 +1091,34 @@
         <v>14</v>
       </c>
     </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H27"/>
+  <autoFilter ref="A1:H28"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the zero-inflated Skellam distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="77">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t xml:space="preserve">zipois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zero-Inflated Skellam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ziskellam</t>
   </si>
 </sst>
 </file>
@@ -378,13 +384,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -1114,6 +1120,84 @@
         <v>21</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding the Laplace distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$28</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$26</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="81">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -146,6 +146,21 @@
     <t xml:space="preserve">geom</t>
   </si>
   <si>
+    <t xml:space="preserve">Laplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean-Scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meanscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real</t>
+  </si>
+  <si>
     <t xml:space="preserve">Multivariate Normal</t>
   </si>
   <si>
@@ -156,9 +171,6 @@
   </si>
   <si>
     <t xml:space="preserve">meanvar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">real</t>
   </si>
   <si>
     <t xml:space="preserve">Multivariate Student‘s t</t>
@@ -384,13 +396,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -724,27 +736,27 @@
         <v>44</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="0" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>44</v>
@@ -760,26 +772,26 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>47</v>
+      <c r="A15" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="E15" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>14</v>
@@ -787,16 +799,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>26</v>
@@ -805,10 +817,10 @@
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,48 +828,48 @@
         <v>51</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>14</v>
@@ -865,25 +877,25 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>14</v>
@@ -891,45 +903,45 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
@@ -943,19 +955,19 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
@@ -964,24 +976,24 @@
         <v>21</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
@@ -995,19 +1007,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>13</v>
@@ -1016,21 +1028,21 @@
         <v>21</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>31</v>
@@ -1042,24 +1054,24 @@
         <v>21</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>13</v>
@@ -1073,16 +1085,16 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>26</v>
@@ -1099,16 +1111,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>26</v>
@@ -1125,19 +1137,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>13</v>
@@ -1146,24 +1158,24 @@
         <v>21</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>63</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>13</v>
@@ -1177,19 +1189,19 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>13</v>
@@ -1198,11 +1210,37 @@
         <v>21</v>
       </c>
       <c r="H31" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H28"/>
+  <autoFilter ref="A1:H29"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the Beta distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$29</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$27</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="88">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -71,6 +71,36 @@
     <t xml:space="preserve">TRUE</t>
   </si>
   <si>
+    <t xml:space="preserve">Beta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean-Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean-Variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meansize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meanvar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Categorical</t>
   </si>
   <si>
@@ -89,9 +119,6 @@
     <t xml:space="preserve">multi</t>
   </si>
   <si>
-    <t xml:space="preserve">FALSE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Double Poisson</t>
   </si>
   <si>
@@ -164,13 +191,7 @@
     <t xml:space="preserve">Multivariate Normal</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean-Variance</t>
-  </si>
-  <si>
     <t xml:space="preserve">mvnorm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meanvar</t>
   </si>
   <si>
     <t xml:space="preserve">Multivariate Student‘s t</t>
@@ -396,13 +417,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.9"/>
   </cols>
@@ -476,10 +497,10 @@
         <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>14</v>
@@ -487,77 +508,77 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
@@ -565,54 +586,54 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="F7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,74 +641,74 @@
         <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>14</v>
@@ -695,51 +716,51 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="E13" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>14</v>
@@ -747,71 +768,71 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="B15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="D15" s="0" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>26</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>13</v>
@@ -825,51 +846,51 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F17" s="0" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="C18" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>14</v>
@@ -877,25 +898,25 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>14</v>
@@ -903,28 +924,28 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="D20" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,74 +953,74 @@
         <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="D21" s="0" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>66</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>14</v>
@@ -1010,74 +1031,74 @@
         <v>69</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>14</v>
@@ -1085,25 +1106,25 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>14</v>
@@ -1111,51 +1132,51 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>14</v>
@@ -1163,84 +1184,162 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="C35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H29"/>
+  <autoFilter ref="A1:H32"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the asymmetric Laplace distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$32</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$33</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="97">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -50,6 +50,30 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
+    <t xml:space="preserve">Asymmetric Laplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean-Scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alaplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meanscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bernoulli</t>
   </si>
   <si>
@@ -65,12 +89,6 @@
     <t xml:space="preserve">binary</t>
   </si>
   <si>
-    <t xml:space="preserve">uni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Beta</t>
   </si>
   <si>
@@ -86,9 +104,6 @@
     <t xml:space="preserve">interval</t>
   </si>
   <si>
-    <t xml:space="preserve">FALSE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mean-Size</t>
   </si>
   <si>
@@ -182,16 +197,7 @@
     <t xml:space="preserve">Laplace</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean-Scale</t>
-  </si>
-  <si>
     <t xml:space="preserve">laplace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meanscale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">real</t>
   </si>
   <si>
     <t xml:space="preserve">Multivariate Normal</t>
@@ -438,13 +444,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -475,7 +481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -498,108 +504,108 @@
         <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="F6" s="0" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
@@ -610,51 +616,51 @@
         <v>30</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,33 +683,33 @@
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>14</v>
@@ -711,51 +717,51 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="D11" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>14</v>
@@ -763,51 +769,51 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="F13" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="F14" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>14</v>
@@ -815,19 +821,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>36</v>
-      </c>
       <c r="E15" s="0" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>13</v>
@@ -836,56 +842,56 @@
         <v>14</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>14</v>
@@ -896,120 +902,120 @@
         <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="F19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="E20" s="0" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="D22" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
@@ -1026,51 +1032,51 @@
         <v>66</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="D24" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="G24" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,74 +1084,74 @@
         <v>71</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="0" t="s">
+      <c r="E26" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="0" t="s">
-        <v>75</v>
-      </c>
       <c r="F26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>14</v>
@@ -1153,28 +1159,28 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,16 +1188,16 @@
         <v>80</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>82</v>
-      </c>
       <c r="D29" s="0" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>13</v>
@@ -1200,56 +1206,56 @@
         <v>14</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="E30" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="F30" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>14</v>
@@ -1260,25 +1266,25 @@
         <v>87</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>88</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,25 +1292,25 @@
         <v>89</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>90</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1312,25 +1318,25 @@
         <v>91</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>92</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1338,81 +1344,107 @@
         <v>93</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="0" t="s">
-        <v>75</v>
-      </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H34"/>
+  <autoFilter ref="A1:H35"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the Birnbaum-Saunders distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$33</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$36</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="99">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -116,6 +116,21 @@
     <t xml:space="preserve">meanvar</t>
   </si>
   <si>
+    <t xml:space="preserve">Birnbaum-Saunders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration</t>
+  </si>
+  <si>
     <t xml:space="preserve">Categorical</t>
   </si>
   <si>
@@ -165,15 +180,6 @@
   </si>
   <si>
     <t xml:space="preserve">rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scale</t>
   </si>
   <si>
     <t xml:space="preserve">Gamma</t>
@@ -444,13 +450,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -625,13 +631,13 @@
         <v>33</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>15</v>
@@ -642,19 +648,19 @@
         <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
@@ -665,25 +671,25 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>15</v>
@@ -712,24 +718,24 @@
         <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
@@ -738,50 +744,50 @@
         <v>15</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="D12" s="0" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="E13" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>13</v>
@@ -790,7 +796,7 @@
         <v>14</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,16 +804,16 @@
         <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>13</v>
@@ -816,24 +822,24 @@
         <v>14</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>13</v>
@@ -842,7 +848,7 @@
         <v>14</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,22 +856,22 @@
         <v>54</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>15</v>
@@ -873,19 +879,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>13</v>
@@ -894,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,16 +908,16 @@
         <v>56</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
@@ -920,7 +926,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,29 +934,29 @@
         <v>58</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="0" t="s">
         <v>60</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -966,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>14</v>
@@ -976,26 +982,26 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="D21" s="0" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>15</v>
@@ -1003,54 +1009,54 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="D23" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,22 +1064,22 @@
         <v>68</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>15</v>
@@ -1081,25 +1087,25 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="D25" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>15</v>
@@ -1110,42 +1116,42 @@
         <v>73</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>75</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="E27" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>13</v>
@@ -1159,19 +1165,19 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>13</v>
@@ -1180,24 +1186,24 @@
         <v>14</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>13</v>
@@ -1214,22 +1220,22 @@
         <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="D30" s="0" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>15</v>
@@ -1237,45 +1243,45 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="0" t="s">
+      <c r="E31" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F31" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
@@ -1284,7 +1290,7 @@
         <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,16 +1298,16 @@
         <v>89</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>90</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>13</v>
@@ -1318,16 +1324,16 @@
         <v>91</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>92</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
@@ -1344,16 +1350,16 @@
         <v>93</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
@@ -1370,16 +1376,16 @@
         <v>95</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
@@ -1388,24 +1394,24 @@
         <v>14</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="0" t="s">
+      <c r="E37" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
@@ -1419,32 +1425,58 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="0" t="s">
+      <c r="C39" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="2" t="s">
+      <c r="E39" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H35"/>
+  <autoFilter ref="A1:H36"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the Burr, Fisk, and Lomax distributions
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$36</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$34</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$39</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$37</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="105">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -131,6 +131,12 @@
     <t xml:space="preserve">duration</t>
   </si>
   <si>
+    <t xml:space="preserve">Burr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Categorical</t>
   </si>
   <si>
@@ -182,6 +188,12 @@
     <t xml:space="preserve">rate</t>
   </si>
   <si>
+    <t xml:space="preserve">Fisk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fisk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gamma</t>
   </si>
   <si>
@@ -204,6 +216,12 @@
   </si>
   <si>
     <t xml:space="preserve">laplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lomax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lomax</t>
   </si>
   <si>
     <t xml:space="preserve">Multivariate Normal</t>
@@ -450,13 +468,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -648,19 +666,19 @@
         <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="D8" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
@@ -671,22 +689,22 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="E9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>14</v>
@@ -697,25 +715,25 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="D10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>15</v>
@@ -723,20 +741,20 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="F11" s="0" t="s">
         <v>13</v>
       </c>
@@ -744,21 +762,21 @@
         <v>15</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>34</v>
@@ -770,21 +788,21 @@
         <v>15</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="D13" s="0" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>34</v>
@@ -793,21 +811,21 @@
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>33</v>
@@ -819,7 +837,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>15</v>
@@ -827,16 +845,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>34</v>
@@ -853,13 +871,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>33</v>
@@ -879,71 +897,71 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
@@ -960,48 +978,48 @@
         <v>60</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="0" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>15</v>
@@ -1012,22 +1030,22 @@
         <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="D22" s="0" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>15</v>
@@ -1035,32 +1053,32 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -1076,10 +1094,10 @@
         <v>12</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>15</v>
@@ -1090,22 +1108,22 @@
         <v>70</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>15</v>
@@ -1113,103 +1131,103 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="D27" s="0" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>15</v>
@@ -1217,19 +1235,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>83</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>13</v>
@@ -1238,50 +1256,50 @@
         <v>14</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>87</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
@@ -1290,24 +1308,24 @@
         <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="D33" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>13</v>
@@ -1321,25 +1339,25 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>92</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>15</v>
@@ -1347,19 +1365,19 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
@@ -1368,7 +1386,7 @@
         <v>14</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,16 +1394,16 @@
         <v>95</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
@@ -1402,16 +1420,16 @@
         <v>97</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>98</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
@@ -1420,24 +1438,24 @@
         <v>14</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>13</v>
@@ -1446,37 +1464,115 @@
         <v>14</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="0" t="s">
+      <c r="C42" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E39" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H39" s="2" t="s">
+      <c r="E42" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H36"/>
+  <autoFilter ref="A1:H39"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the logistic distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$39</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$37</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$41</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="109">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -212,10 +212,22 @@
     <t xml:space="preserve">geom</t>
   </si>
   <si>
+    <t xml:space="preserve">Kumaraswamy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuma</t>
+  </si>
+  <si>
     <t xml:space="preserve">Laplace</t>
   </si>
   <si>
     <t xml:space="preserve">laplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logistic</t>
   </si>
   <si>
     <t xml:space="preserve">Lomax</t>
@@ -468,13 +480,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -1004,22 +1016,22 @@
         <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>15</v>
@@ -1030,22 +1042,22 @@
         <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>15</v>
@@ -1056,45 +1068,45 @@
         <v>66</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="0" t="s">
         <v>68</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>14</v>
@@ -1108,51 +1120,51 @@
         <v>70</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="B26" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,16 +1172,16 @@
         <v>74</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>13</v>
@@ -1183,45 +1195,45 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>77</v>
-      </c>
       <c r="D28" s="0" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>80</v>
-      </c>
       <c r="D29" s="0" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>13</v>
@@ -1235,71 +1247,71 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="D30" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="F30" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
@@ -1308,25 +1320,25 @@
         <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="C33" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="F33" s="0" t="s">
         <v>13</v>
       </c>
@@ -1334,30 +1346,30 @@
         <v>14</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>15</v>
@@ -1365,19 +1377,19 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
@@ -1386,30 +1398,30 @@
         <v>14</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>15</v>
@@ -1417,19 +1429,19 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
@@ -1438,7 +1450,7 @@
         <v>14</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1446,16 +1458,16 @@
         <v>99</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>100</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>13</v>
@@ -1498,16 +1510,16 @@
         <v>103</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>104</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>13</v>
@@ -1516,24 +1528,24 @@
         <v>14</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>13</v>
@@ -1542,37 +1554,89 @@
         <v>14</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D42" s="0" t="s">
+      <c r="C44" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E42" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="2" t="s">
+      <c r="E44" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H39"/>
+  <autoFilter ref="A1:H41"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the Kumaraswamy distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -483,10 +483,10 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>

</xml_diff>

<commit_message>
Adding the Rayleigh distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$41</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$39</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$40</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="111">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t xml:space="preserve">pois</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rayleigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rayleigh</t>
   </si>
   <si>
     <t xml:space="preserve">Skellam</t>
@@ -480,13 +486,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -1302,42 +1308,42 @@
         <v>85</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="D32" s="0" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="0" t="s">
+      <c r="E33" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>13</v>
@@ -1351,19 +1357,19 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
@@ -1372,24 +1378,24 @@
         <v>14</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
@@ -1406,22 +1412,22 @@
         <v>94</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="D36" s="0" t="s">
-        <v>97</v>
+        <v>29</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>15</v>
@@ -1429,42 +1435,42 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="0" t="s">
+      <c r="E37" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>34</v>
@@ -1476,7 +1482,7 @@
         <v>14</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,16 +1490,16 @@
         <v>101</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>102</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>13</v>
@@ -1510,13 +1516,13 @@
         <v>103</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>104</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>49</v>
@@ -1536,13 +1542,13 @@
         <v>105</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>106</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>49</v>
@@ -1562,16 +1568,16 @@
         <v>107</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>108</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>13</v>
@@ -1580,24 +1586,24 @@
         <v>14</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="0" t="s">
+      <c r="E43" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>13</v>
@@ -1611,32 +1617,58 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" s="0" t="s">
+      <c r="C45" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="2" t="s">
+      <c r="E45" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H41"/>
+  <autoFilter ref="A1:H42"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the log-normal distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$40</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$43</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$41</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="115">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t xml:space="preserve">laplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log-Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log-Mean-Variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lognorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logmeanvar</t>
   </si>
   <si>
     <t xml:space="preserve">Logistic</t>
@@ -486,13 +498,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -1074,16 +1086,16 @@
         <v>66</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
@@ -1097,25 +1109,25 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>15</v>
@@ -1123,22 +1135,22 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>14</v>
@@ -1148,14 +1160,14 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>72</v>
+      <c r="A26" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>29</v>
@@ -1174,26 +1186,26 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>74</v>
+      <c r="A27" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>15</v>
@@ -1201,16 +1213,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>49</v>
@@ -1219,10 +1231,10 @@
         <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,48 +1242,48 @@
         <v>78</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>15</v>
@@ -1279,25 +1291,25 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>15</v>
@@ -1305,19 +1317,19 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
@@ -1331,45 +1343,45 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>92</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
@@ -1383,19 +1395,19 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
@@ -1404,24 +1416,24 @@
         <v>14</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
@@ -1435,25 +1447,25 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>15</v>
@@ -1461,42 +1473,42 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>102</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>34</v>
@@ -1508,24 +1520,24 @@
         <v>14</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>13</v>
@@ -1539,16 +1551,16 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>49</v>
@@ -1565,16 +1577,16 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>49</v>
@@ -1591,19 +1603,19 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>13</v>
@@ -1612,24 +1624,24 @@
         <v>14</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>92</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>13</v>
@@ -1643,32 +1655,58 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" s="0" t="s">
+      <c r="C46" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E45" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H45" s="2" t="s">
+      <c r="E46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H42"/>
+  <autoFilter ref="A1:H43"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the logit-normal distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$41</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="119">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -240,6 +240,18 @@
   </si>
   <si>
     <t xml:space="preserve">logistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logit-Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logit-Mean-Variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logitnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logitmeanvar</t>
   </si>
   <si>
     <t xml:space="preserve">Lomax</t>
@@ -498,13 +510,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -1138,22 +1150,22 @@
         <v>72</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>15</v>
@@ -1161,22 +1173,22 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>14</v>
@@ -1186,14 +1198,14 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>76</v>
+      <c r="A27" s="0" t="s">
+        <v>78</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>29</v>
@@ -1212,26 +1224,26 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>78</v>
+      <c r="A28" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>15</v>
@@ -1239,16 +1251,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>49</v>
@@ -1257,10 +1269,10 @@
         <v>13</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,48 +1280,48 @@
         <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>15</v>
@@ -1317,25 +1329,25 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>15</v>
@@ -1343,19 +1355,19 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>13</v>
@@ -1369,45 +1381,45 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
@@ -1421,19 +1433,19 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
@@ -1442,24 +1454,24 @@
         <v>14</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
@@ -1473,25 +1485,25 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>15</v>
@@ -1499,42 +1511,42 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>106</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>34</v>
@@ -1546,24 +1558,24 @@
         <v>14</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>13</v>
@@ -1577,16 +1589,16 @@
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>49</v>
@@ -1603,16 +1615,16 @@
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>49</v>
@@ -1629,19 +1641,19 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>13</v>
@@ -1650,24 +1662,24 @@
         <v>14</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>96</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>13</v>
@@ -1681,32 +1693,58 @@
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D46" s="0" t="s">
+      <c r="C47" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H46" s="2" t="s">
+      <c r="E47" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H43"/>
+  <autoFilter ref="A1:H47"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the exponential-logarithmic distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$47</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$42</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$43</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="121">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t xml:space="preserve">rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exponential-Logarithmic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">explog</t>
   </si>
   <si>
     <t xml:space="preserve">Fisk</t>
@@ -510,13 +516,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -864,13 +870,13 @@
         <v>54</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>34</v>
@@ -879,7 +885,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>15</v>
@@ -890,13 +896,13 @@
         <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>34</v>
@@ -905,24 +911,24 @@
         <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>34</v>
@@ -934,7 +940,7 @@
         <v>14</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,13 +948,13 @@
         <v>58</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>34</v>
@@ -960,21 +966,21 @@
         <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>34</v>
@@ -986,7 +992,7 @@
         <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,22 +1000,22 @@
         <v>60</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>15</v>
@@ -1017,16 +1023,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>49</v>
@@ -1038,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,25 +1052,25 @@
         <v>62</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,22 +1078,22 @@
         <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>15</v>
@@ -1098,16 +1104,16 @@
         <v>66</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="D23" s="0" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
@@ -1121,19 +1127,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E24" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>13</v>
@@ -1150,16 +1156,16 @@
         <v>72</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>74</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>13</v>
@@ -1173,25 +1179,25 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="0" t="s">
+      <c r="D26" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E26" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>15</v>
@@ -1202,19 +1208,19 @@
         <v>78</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>79</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>14</v>
@@ -1224,7 +1230,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="0" t="s">
         <v>80</v>
       </c>
       <c r="B28" s="0" t="s">
@@ -1250,26 +1256,26 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="D29" s="0" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>15</v>
@@ -1277,16 +1283,16 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>49</v>
@@ -1295,36 +1301,36 @@
         <v>13</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="D31" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,22 +1338,22 @@
         <v>88</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>89</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>15</v>
@@ -1355,25 +1361,25 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="F33" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>15</v>
@@ -1384,16 +1390,16 @@
         <v>93</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>13</v>
@@ -1410,42 +1416,42 @@
         <v>95</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="D35" s="0" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
@@ -1459,19 +1465,19 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
@@ -1480,24 +1486,24 @@
         <v>14</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>13</v>
@@ -1514,22 +1520,22 @@
         <v>104</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="D39" s="0" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>15</v>
@@ -1537,42 +1543,42 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="0" t="s">
+      <c r="E40" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="F40" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>34</v>
@@ -1584,7 +1590,7 @@
         <v>14</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,16 +1598,16 @@
         <v>111</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>112</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>13</v>
@@ -1618,13 +1624,13 @@
         <v>113</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>114</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="E43" s="0" t="s">
         <v>49</v>
@@ -1644,13 +1650,13 @@
         <v>115</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>116</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>49</v>
@@ -1670,16 +1676,16 @@
         <v>117</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>118</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>13</v>
@@ -1688,24 +1694,24 @@
         <v>14</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D46" s="0" t="s">
+      <c r="E46" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>13</v>
@@ -1719,32 +1725,58 @@
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D47" s="0" t="s">
+      <c r="C48" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E47" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H47" s="2" t="s">
+      <c r="E48" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H47"/>
+  <autoFilter ref="A1:H48"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Adding the generalized error distribution
</commit_message>
<xml_diff>
--- a/data-raw/distr_table.xlsx
+++ b/data-raw/distr_table.xlsx
@@ -11,8 +11,8 @@
     <sheet name="dist_table" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$48</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$43</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">dist_table!$A$1:$H$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">dist_table!$A$1:$H$44</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="123">
   <si>
     <t xml:space="preserve">distr_title</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t xml:space="preserve">gamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generalized Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ged</t>
   </si>
   <si>
     <t xml:space="preserve">Generalized Gamma</t>
@@ -516,13 +522,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.86"/>
   </cols>
@@ -974,16 +980,16 @@
         <v>60</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>61</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>13</v>
@@ -992,21 +998,21 @@
         <v>14</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>34</v>
@@ -1018,7 +1024,7 @@
         <v>14</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,22 +1032,22 @@
         <v>62</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>15</v>
@@ -1049,16 +1055,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>49</v>
@@ -1070,7 +1076,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,25 +1084,25 @@
         <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,22 +1110,22 @@
         <v>66</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>15</v>
@@ -1130,16 +1136,16 @@
         <v>68</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>70</v>
-      </c>
       <c r="D24" s="0" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>13</v>
@@ -1153,19 +1159,19 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="E25" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>13</v>
@@ -1182,16 +1188,16 @@
         <v>74</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>76</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>13</v>
@@ -1205,25 +1211,25 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="D27" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="E27" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>15</v>
@@ -1234,19 +1240,19 @@
         <v>80</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>14</v>
@@ -1256,7 +1262,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="0" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="0" t="s">
@@ -1282,26 +1288,26 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="D30" s="0" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>15</v>
@@ -1309,16 +1315,16 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>49</v>
@@ -1327,36 +1333,36 @@
         <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="D32" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,22 +1370,22 @@
         <v>90</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>91</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>15</v>
@@ -1387,25 +1393,25 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="0" t="s">
+      <c r="D34" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="F34" s="0" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>15</v>
@@ -1416,16 +1422,16 @@
         <v>95</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>96</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>13</v>
@@ -1442,42 +1448,42 @@
         <v>97</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="D36" s="0" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="0" t="s">
+      <c r="E37" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>13</v>
@@ -1491,19 +1497,19 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>13</v>
@@ -1512,24 +1518,24 @@
         <v>14</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>13</v>
@@ -1546,22 +1552,22 @@
         <v>106</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="D40" s="0" t="s">
-        <v>109</v>
+        <v>29</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="F40" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>15</v>
@@ -1569,42 +1575,42 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="0" t="s">
+      <c r="E41" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>34</v>
-      </c>
       <c r="F41" s="0" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>34</v>
@@ -1616,7 +1622,7 @@
         <v>14</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,16 +1630,16 @@
         <v>113</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>114</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>13</v>
@@ -1650,13 +1656,13 @@
         <v>115</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>116</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>49</v>
@@ -1676,13 +1682,13 @@
         <v>117</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>118</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>49</v>
@@ -1702,16 +1708,16 @@
         <v>119</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>120</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>13</v>
@@ -1720,24 +1726,24 @@
         <v>14</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" s="0" t="s">
+      <c r="E47" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>13</v>
@@ -1751,32 +1757,58 @@
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D48" s="0" t="s">
+      <c r="C49" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="2" t="s">
+      <c r="E49" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H48"/>
+  <autoFilter ref="A1:H49"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>